<commit_message>
Individual project and Exercise 6,7
</commit_message>
<xml_diff>
--- a/projects/project_anushan/e_draft_presentation/draft/feedback_Pitch your project (v2).xlsx
+++ b/projects/project_anushan/e_draft_presentation/draft/feedback_Pitch your project (v2).xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20382"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Applied Macro\Projects\projects\project_anushan\e_draft_presentation\draft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Applied Macro\Projects\projects\project_anushan\e_draft_presentation\draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866D0E79-213B-404B-A4AE-4C98A1D4CF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4581E46-94A4-493F-A413-C9B1F13EA316}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="26295" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
-    <sheet name="Migration numbers " sheetId="2" r:id="rId3"/>
-    <sheet name="Figures" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Migration numbers " sheetId="2" r:id="rId4"/>
+    <sheet name="Figures" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Donnerstag, 3. November 2022, 13:41</t>
   </si>
@@ -97,42 +98,90 @@
     <t>Rainer Kotschy and Uwe Sunde, (2018) Can education compensate the effect of population ageing on macroeconomic performance?</t>
   </si>
   <si>
-    <t xml:space="preserve">What is the impact of (demographic factors such as aging and) labour migration and, education investments on the macrpeconomic performance of South Asian countries?
+    <t xml:space="preserve">Same graph with South Asian Countries </t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Projected development paths of countries around the world until 2050, and for a quantitative assessment of different scenarios of ageing and education acquisition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, I plan on using casual identification to understand the impact of education and age dynamics on the macroeconomic performance (Output per capita). The estimates allow to conduct counterfactual simulations of economic performance under alternative scenarios of ageing, labour migration, human capital dynamics, labour force participation, and productivity. </t>
+  </si>
+  <si>
+    <t>Panel data analysis with dummy variables for age wise productivity measure and controls for country specific fixed effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel data with country level and time </t>
+  </si>
+  <si>
+    <t>Load data and run regression - 19 Nov
+conduct quantitative exercise based on data - 25 Nov
+Finish Analysis (including preparing slides) - 2 Dec
+Additional time to finalise - 9 Dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4012 observations for 120 countries </t>
+  </si>
+  <si>
+    <t>codebook countrz</t>
+  </si>
+  <si>
+    <t>AustraliaAustriaBelgiumCanadaChileColombiaCosta RicaCzech RepublicDenmarkEstonia</t>
+  </si>
+  <si>
+    <t>FinlandFranceGermanyGreeceHungaryIcelandIrelandIsraelItalyJapan</t>
+  </si>
+  <si>
+    <r>
+      <t>KoreaLatvia</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0B1E2D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Lithuania</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0B1E2D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>LuxembourgMexicoNetherlandsNew ZealandNorwayPolandPortugal</t>
+    </r>
+  </si>
+  <si>
+    <t>Slovak RepublicSloveniaSpainSwedenSwitzerlandTürkiyeUnited KingdomUnited States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, but not concertly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is an estimated 272 million international migrants around the world accounting for 3.5% of the world population. 40% of the migrants are of age between 25 to 45. The loss of this working age population can  negatively impact the productive potential of a country. Therefore in this study, in addition to the usual population aging, I factor in the demographic change in the population due to an estimated migration away from the country of origin.  Further, the study also aims to understand how the investments in education can compensate for the loss due to migration and aging. The paper is also particularly focussed on developing countries as they account for a higher share of labour migration in the world. </t>
+  </si>
+  <si>
+    <t>ln (yit) = a*ln(yit-1) + b*ln(kit) + (1-b)c*(Sit)+ (1-b)c*Sigma(Sit)+ di+Tt+eit</t>
+  </si>
+  <si>
+    <t>long panel data set for more than 120 countries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the impact of demographic factors such as aging and labour migration and, education investments on the macroeconomic performance of developing countries?
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is an estimated 272 million international migrants around the world accounting for 3.5% of the world population. 40% of the migrants are of age between 25 to 45. The loss of this working age population can  negatively impact the productive potential of a country. Therefore in this study, in addition to the usual population aging, I factor in the demographic change in the population due to an estimated migration away from the country of origin.  Further, the study also aims to understand how the investments in education can compensate for the loss due to migration. The paper is also particularly focussed on developing South Asian countries as they account for a higher share of labour migration in the world. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Same graph with South Asian Countries </t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Projected development paths of countries around the world until 2050, and for a quantitative assessment of different scenarios of ageing and education acquisition.</t>
-  </si>
-  <si>
-    <t>long panel data set for more than 130 countries.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, I plan on using casual identification to understand the impact of education and age dynamics on the macroeconomic performance (Output per capita). The estimates allow to conduct counterfactual simulations of economic performance under alternative scenarios of ageing, labour migration, human capital dynamics, labour force participation, and productivity. </t>
-  </si>
-  <si>
-    <t>Panel data analysis with dummy variables for age wise productivity measure and controls for country specific fixed effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ln (yit) = a*ln(yit-1) + b*ln(kit) + (1-b) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panel data with country level and time </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -176,6 +225,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0B1E2D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0B1E2D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -198,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -222,6 +284,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -245,15 +310,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>32924</xdr:colOff>
+      <xdr:colOff>5747924</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>155276</xdr:rowOff>
+      <xdr:rowOff>312932</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5639177</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>988349</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>879894</xdr:rowOff>
+      <xdr:rowOff>1037550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -276,7 +341,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="723037" y="7013276"/>
+          <a:off x="6417958" y="7538794"/>
           <a:ext cx="5606253" cy="724618"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -755,32 +820,32 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="95.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="95.5703125" style="3" customWidth="1"/>
     <col min="3" max="21" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -791,26 +856,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.55" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="132.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="132.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -819,7 +884,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>23</v>
       </c>
@@ -830,9 +895,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -841,9 +906,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>31</v>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -864,9 +929,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="106.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>32</v>
+    <row r="21" spans="1:2" ht="106.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,6 +940,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="5" t="s">
@@ -883,18 +953,18 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>33</v>
+      <c r="B27" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -903,10 +973,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="5" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -915,20 +990,31 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="5" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="3">
+        <f>120-38</f>
+        <v>82</v>
+      </c>
+    </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -939,18 +1025,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{848DDECA-FCD7-4C97-BDF3-D2C05982A997}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F67173-3FEC-44C8-A008-C7F6C52643BA}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9979789F-6AA9-4BFB-93BC-6676921C7375}">
   <dimension ref="A2:I33"/>
   <sheetViews>
@@ -958,7 +1088,7 @@
       <selection activeCell="AA31" sqref="AA31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -980,7 +1110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBAB1C0-5D03-4E31-AD19-A369CDE84FFE}">
   <dimension ref="A2"/>
   <sheetViews>
@@ -988,11 +1118,11 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>